<commit_message>
added to maintenance report data
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\Documents\DS_Projects\AptComplex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{11E2C56D-AD61-4602-B7B3-B9042A68D096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F53B22-69D2-4FCE-9F75-0751B4BFF353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F6C36B38-7868-4ED7-9EEA-CAD4855C7B4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tickets Open" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="32">
   <si>
     <t>Unit</t>
   </si>
@@ -60,6 +61,78 @@
   </si>
   <si>
     <t>Cost</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Master Bedroom</t>
+  </si>
+  <si>
+    <t>Bedroom</t>
+  </si>
+  <si>
+    <t>Master Bath</t>
+  </si>
+  <si>
+    <t>Bath</t>
+  </si>
+  <si>
+    <t>Kitchen</t>
+  </si>
+  <si>
+    <t>Living Room</t>
+  </si>
+  <si>
+    <t>Washer/Dryer</t>
+  </si>
+  <si>
+    <t>Plumbing</t>
+  </si>
+  <si>
+    <t>Electrical</t>
+  </si>
+  <si>
+    <t>Appliance</t>
+  </si>
+  <si>
+    <t>Flooring</t>
+  </si>
+  <si>
+    <t>Walls/Ceiling</t>
+  </si>
+  <si>
+    <t>A/C</t>
+  </si>
+  <si>
+    <t>Doors</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Pest</t>
+  </si>
+  <si>
+    <t>PointOfContact</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Windows</t>
+  </si>
+  <si>
+    <t>Countertops</t>
   </si>
 </sst>
 </file>
@@ -95,8 +168,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,19 +505,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0198A74-2471-4896-9AB2-3658FCD6C937}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,332 +541,927 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>103</v>
       </c>
-      <c r="H2">
+      <c r="B2" s="1">
+        <v>45835</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1">
+        <v>45844</v>
+      </c>
+      <c r="K2">
         <v>1351</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>112</v>
       </c>
-      <c r="H3">
+      <c r="B3" s="1">
+        <v>45773</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="1">
+        <v>45858</v>
+      </c>
+      <c r="K3">
         <v>570</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>107</v>
       </c>
-      <c r="H4">
+      <c r="B4" s="1">
+        <v>45781</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4">
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>107</v>
       </c>
-      <c r="H5">
+      <c r="B5" s="1">
+        <v>45808</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="1">
+        <v>45834</v>
+      </c>
+      <c r="K5">
         <v>685</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>103</v>
       </c>
-      <c r="H6">
+      <c r="B6" s="1">
+        <v>45782</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="1">
+        <v>45856</v>
+      </c>
+      <c r="K6">
         <v>261</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>114</v>
       </c>
-      <c r="H7">
+      <c r="B7" s="1">
+        <v>45784</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="1">
+        <v>45814</v>
+      </c>
+      <c r="K7">
         <v>550</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>102</v>
       </c>
-      <c r="H8">
+      <c r="B8" s="1">
+        <v>45669</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="1">
+        <v>45692</v>
+      </c>
+      <c r="K8">
         <v>432</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>104</v>
       </c>
-      <c r="H9">
+      <c r="B9" s="1">
+        <v>45821</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="1">
+        <v>45841</v>
+      </c>
+      <c r="K9">
         <v>364</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>112</v>
       </c>
-      <c r="H10">
+      <c r="B10" s="1">
+        <v>45749</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10">
         <v>578</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>115</v>
       </c>
-      <c r="H11">
+      <c r="B11" s="1">
+        <v>45825</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="1">
+        <v>45839</v>
+      </c>
+      <c r="K11">
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>115</v>
       </c>
-      <c r="H12">
+      <c r="B12" s="1">
+        <v>45800</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="1">
+        <v>45852</v>
+      </c>
+      <c r="K12">
         <v>429</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>113</v>
       </c>
-      <c r="H13">
+      <c r="B13" s="1">
+        <v>45763</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="1">
+        <v>45840</v>
+      </c>
+      <c r="K13">
         <v>356</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>114</v>
       </c>
-      <c r="H14">
+      <c r="B14" s="1">
+        <v>45698</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="1">
+        <v>45863</v>
+      </c>
+      <c r="K14">
         <v>436</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>101</v>
       </c>
-      <c r="H15">
+      <c r="B15" s="1">
+        <v>45786</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="1">
+        <v>45842</v>
+      </c>
+      <c r="K15">
         <v>357</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>107</v>
       </c>
-      <c r="H16">
+      <c r="B16" s="1">
+        <v>45737</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="1">
+        <v>45757</v>
+      </c>
+      <c r="K16">
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>102</v>
       </c>
-      <c r="H17">
+      <c r="B17" s="1">
+        <v>45701</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="1"/>
+      <c r="K17">
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>112</v>
       </c>
-      <c r="H18">
+      <c r="B18" s="1">
+        <v>45798</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="1">
+        <v>45820</v>
+      </c>
+      <c r="K18">
         <v>360</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>113</v>
       </c>
-      <c r="H19">
+      <c r="B19" s="1">
+        <v>45756</v>
+      </c>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="1">
+        <v>45840</v>
+      </c>
+      <c r="K19">
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>108</v>
       </c>
-      <c r="H20">
+      <c r="B20" s="1">
+        <v>45747</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="J20" s="1">
+        <v>45858</v>
+      </c>
+      <c r="K20">
         <v>729</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>106</v>
       </c>
-      <c r="H21">
+      <c r="B21" s="1">
+        <v>45817</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" s="1"/>
+      <c r="K21">
         <v>747</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>107</v>
       </c>
-      <c r="H22">
+      <c r="B22" s="1">
+        <v>45740</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" s="1"/>
+      <c r="K22">
         <v>652</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>108</v>
       </c>
-      <c r="H23">
+      <c r="B23" s="1">
+        <v>45728</v>
+      </c>
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="J23" s="1">
+        <v>45752</v>
+      </c>
+      <c r="K23">
         <v>501</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>106</v>
       </c>
-      <c r="H24">
+      <c r="B24" s="1">
+        <v>45773</v>
+      </c>
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+      <c r="J24" s="1">
+        <v>45797</v>
+      </c>
+      <c r="K24">
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>105</v>
       </c>
-      <c r="H25">
+      <c r="B25" s="1">
+        <v>45697</v>
+      </c>
+      <c r="C25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="J25" s="1">
+        <v>45786</v>
+      </c>
+      <c r="K25">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>114</v>
       </c>
-      <c r="H26">
+      <c r="B26" s="1">
+        <v>45711</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J26" s="1">
+        <v>45714</v>
+      </c>
+      <c r="K26">
         <v>221</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>109</v>
       </c>
-      <c r="H27">
+      <c r="B27" s="1">
+        <v>45776</v>
+      </c>
+      <c r="C27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" t="s">
+        <v>9</v>
+      </c>
+      <c r="J27" s="1"/>
+      <c r="K27">
         <v>597</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>104</v>
       </c>
-      <c r="H28">
+      <c r="B28" s="1">
+        <v>45663</v>
+      </c>
+      <c r="C28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="J28" s="1">
+        <v>45782</v>
+      </c>
+      <c r="K28">
         <v>424</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>101</v>
       </c>
-      <c r="H29">
+      <c r="B29" s="1">
+        <v>45835</v>
+      </c>
+      <c r="C29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" t="s">
+        <v>9</v>
+      </c>
+      <c r="J29" s="1">
+        <v>45837</v>
+      </c>
+      <c r="K29">
         <v>334</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>114</v>
       </c>
-      <c r="H30">
+      <c r="B30" s="1">
+        <v>45659</v>
+      </c>
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="J30" s="1">
+        <v>45669</v>
+      </c>
+      <c r="K30">
         <v>235</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>104</v>
       </c>
-      <c r="H31">
+      <c r="B31" s="1">
+        <v>45775</v>
+      </c>
+      <c r="C31" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" t="s">
+        <v>11</v>
+      </c>
+      <c r="J31" s="1"/>
+      <c r="K31">
         <v>619</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>107</v>
       </c>
-      <c r="H32">
+      <c r="B32" s="1">
+        <v>45750</v>
+      </c>
+      <c r="C32" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+      <c r="J32" s="1">
+        <v>45843</v>
+      </c>
+      <c r="K32">
         <v>333</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>103</v>
       </c>
-      <c r="H33">
+      <c r="B33" s="1">
+        <v>45833</v>
+      </c>
+      <c r="C33" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" t="s">
+        <v>9</v>
+      </c>
+      <c r="J33" s="1">
+        <v>45843</v>
+      </c>
+      <c r="K33">
         <v>520</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>101</v>
       </c>
-      <c r="H34">
+      <c r="B34" s="1">
+        <v>45823</v>
+      </c>
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" t="s">
+        <v>11</v>
+      </c>
+      <c r="J34" s="1">
+        <v>45851</v>
+      </c>
+      <c r="K34">
         <v>732</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>109</v>
       </c>
-      <c r="H35">
+      <c r="B35" s="1">
+        <v>45660</v>
+      </c>
+      <c r="C35" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" t="s">
+        <v>9</v>
+      </c>
+      <c r="J35" s="1">
+        <v>45841</v>
+      </c>
+      <c r="K35">
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>101</v>
       </c>
-      <c r="H36">
+      <c r="B36" s="1">
+        <v>45694</v>
+      </c>
+      <c r="C36" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" t="s">
+        <v>10</v>
+      </c>
+      <c r="J36" s="1">
+        <v>45765</v>
+      </c>
+      <c r="K36">
         <v>584</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>111</v>
       </c>
-      <c r="H37">
+      <c r="B37" s="1">
+        <v>45787</v>
+      </c>
+      <c r="C37" t="s">
+        <v>26</v>
+      </c>
+      <c r="D37" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+      <c r="J37" s="1">
+        <v>45823</v>
+      </c>
+      <c r="K37">
         <v>261</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>108</v>
       </c>
-      <c r="H38">
+      <c r="B38" s="1">
+        <v>45708</v>
+      </c>
+      <c r="C38" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+      <c r="J38" s="1">
+        <v>45717</v>
+      </c>
+      <c r="K38">
         <v>206</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>103</v>
       </c>
-      <c r="H39">
+      <c r="B39" s="1">
+        <v>45679</v>
+      </c>
+      <c r="C39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" t="s">
+        <v>9</v>
+      </c>
+      <c r="J39" s="1">
+        <v>45705</v>
+      </c>
+      <c r="K39">
         <v>84</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>114</v>
       </c>
-      <c r="H40">
+      <c r="B40" s="1">
+        <v>45735</v>
+      </c>
+      <c r="C40" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" t="s">
+        <v>10</v>
+      </c>
+      <c r="J40" s="1">
+        <v>45775</v>
+      </c>
+      <c r="K40">
         <v>193</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>101</v>
       </c>
-      <c r="H41">
+      <c r="B41" s="1">
+        <v>45766</v>
+      </c>
+      <c r="C41" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" t="s">
+        <v>9</v>
+      </c>
+      <c r="J41" s="1">
+        <v>45779</v>
+      </c>
+      <c r="K41">
         <v>517</v>
       </c>
     </row>
@@ -793,4 +1469,258 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A30813-153B-4695-895C-A2205CB495C1}">
+  <dimension ref="A2:E41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>